<commit_message>
fix 5.45 barrels and velocities
</commit_message>
<xml_diff>
--- a/changes/545-barrels.xlsx
+++ b/changes/545-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3E32AB-6A30-4059-BF56-932038DF0A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38896AF0-DF03-44A5-B2E9-C7D83B1B746A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -959,7 +959,7 @@
   <dimension ref="A1:V39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,7 +1061,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <f>C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300</f>
@@ -1148,20 +1148,20 @@
         <v>24</v>
       </c>
       <c r="C5" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1">
         <v>0.28000000000000003</v>
       </c>
       <c r="E5" s="1">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="I5" s="1">
         <v>-0.1</v>
@@ -1176,7 +1176,7 @@
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>2.1333333333333333</v>
+        <v>-1.3166666666666673</v>
       </c>
       <c r="P5">
         <v>0.04</v>

</xml_diff>

<commit_message>
random ahh adjustments (mostly smgs)
</commit_message>
<xml_diff>
--- a/changes/545-barrels.xlsx
+++ b/changes/545-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3403908-5D12-4A81-9371-53204818BC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047A79F7-9642-40DB-8649-DB3A1FEA2F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -977,7 +977,7 @@
   <dimension ref="A1:V39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1182,7 @@
         <v>0.25</v>
       </c>
       <c r="I5" s="1">
-        <v>-0.1</v>
+        <v>-0.08</v>
       </c>
       <c r="J5" s="1">
         <v>-200</v>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>-1.5166666666666666</v>
+        <v>-1.3166666666666664</v>
       </c>
       <c r="P5">
         <v>0.08</v>
@@ -1355,7 +1355,7 @@
         <v>0.15</v>
       </c>
       <c r="I9" s="1">
-        <v>-0.1</v>
+        <v>-0.05</v>
       </c>
       <c r="J9" s="1">
         <v>-90</v>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>-14.850000000000001</v>
+        <v>-14.350000000000001</v>
       </c>
       <c r="P9">
         <v>0.33</v>

</xml_diff>